<commit_message>
-fix lỗi khi đồng bộ android
</commit_message>
<xml_diff>
--- a/filedatabase/lopmonhoc.xlsx
+++ b/filedatabase/lopmonhoc.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>tenLopMonHoc</t>
   </si>
@@ -55,6 +55,15 @@
   </si>
   <si>
     <t>vietha</t>
+  </si>
+  <si>
+    <t>INT2204 1</t>
+  </si>
+  <si>
+    <t>Hương đối tượng</t>
+  </si>
+  <si>
+    <t>Tô Văn Khánh</t>
   </si>
 </sst>
 </file>
@@ -102,6 +111,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -149,7 +161,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -184,7 +196,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -393,10 +405,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D3:H6"/>
+  <dimension ref="D3:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -467,6 +479,20 @@
         <v>12</v>
       </c>
     </row>
+    <row r="7" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>